<commit_message>
Added Entities, Updated SQL script, converted Log to CSV
</commit_message>
<xml_diff>
--- a/Log_Document/Log_book.xlsx
+++ b/Log_Document/Log_book.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="58">
   <si>
     <t>Date</t>
   </si>
@@ -187,6 +187,9 @@
   </si>
   <si>
     <t>End of june exams</t>
+  </si>
+  <si>
+    <t>Updated domain objects, refine SQL, converted log to CSV, Created entities</t>
   </si>
 </sst>
 </file>
@@ -194,8 +197,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="167" formatCode="[$-409]h:mm\ AM/PM;@"/>
-    <numFmt numFmtId="168" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="164" formatCode="[$-409]h:mm\ AM/PM;@"/>
+    <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -228,8 +231,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -533,8 +536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:E644"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="D115" sqref="D115"/>
+    <sheetView tabSelected="1" topLeftCell="B142" workbookViewId="0">
+      <selection activeCell="D157" sqref="D157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1851,6 +1854,12 @@
         <v>41812</v>
       </c>
       <c r="C157" s="1"/>
+      <c r="D157" t="s">
+        <v>57</v>
+      </c>
+      <c r="E157" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="158" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B158" s="2">

</xml_diff>